<commit_message>
Fixed minor mistakes in the XPATHs of the Conceptual Mappings
</commit_message>
<xml_diff>
--- a/mappings/package_F13/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F13/transformation/conceptual_mappings.xlsx
@@ -54,7 +54,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>4.0.0</t>
+    <t>4.0.1</t>
   </si>
   <si>
     <r>
@@ -2748,7 +2748,7 @@
     <t>Received Submissions Count</t>
   </si>
   <si>
-    <t>RESULTS/AWARDED_PRIZE/NB_PARTICIPANTS</t>
+    <t>RESULTS/AWARDED_PRIZE/PARTICIPANTS/NB_PARTICIPANTS</t>
   </si>
   <si>
     <t xml:space="preserve"> epo:SubmissionStatisticalInformation / xsd:integer</t>
@@ -2763,7 +2763,7 @@
     <t>Number of participating SMEs</t>
   </si>
   <si>
-    <t>RESULTS/AWARDED_PRIZE/NB_PARTICIPANTS_SME</t>
+    <t>RESULTS/AWARDED_PRIZE/PARTICIPANTS/NB_PARTICIPANTS_SME</t>
   </si>
   <si>
     <t>epo:SubmissionStatisticalInformation / xsd:integer</t>
@@ -2803,7 +2803,7 @@
     <t>Number of participants from other countries</t>
   </si>
   <si>
-    <t>RESULTS/AWARDED_PRIZE/NB_PARTICIPANTS_OTHER_EU</t>
+    <t>RESULTS/AWARDED_PRIZE/PARTICIPANTS/NB_PARTICIPANTS_OTHER_EU</t>
   </si>
   <si>
     <r>
@@ -2962,7 +2962,7 @@
     <t>V.3.3.3</t>
   </si>
   <si>
-    <t>RESULTS/AWARDED_PRIZE/WINNERS/WINNER\ADDRESS_WINNER/ADDRESS</t>
+    <t>RESULTS/AWARDED_PRIZE/WINNERS/WINNER/ADDRESS_WINNER/ADDRESS</t>
   </si>
   <si>
     <r>

</xml_diff>

<commit_message>
Generated output for packages F13, F20 and F23, based on CM v 5.5.0 ready for TX1.3 delivery.
</commit_message>
<xml_diff>
--- a/mappings/package_F13/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F13/transformation/conceptual_mappings.xlsx
@@ -54,7 +54,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>5.4.0</t>
+    <t>5.5.0</t>
   </si>
   <si>
     <r>
@@ -2694,7 +2694,7 @@
     <t>epo:LotAwardOutcome / epo:TenderAwardOutcome / epo:Winner</t>
   </si>
   <si>
-    <t>?this epo:comprisesTenderAwardOutcome / epo:awardsLotToWinner ?value</t>
+    <t>?this epo:comprisesTenderAwardOutcome / epo:indicatesAwardOfLotToWinner ?value</t>
   </si>
   <si>
     <t>V.3.1</t>

</xml_diff>

<commit_message>
Updated CM to v6.6.0 to reflect start XSD version R2.0.9.S01.E01 and start date 2014-01-01. Also generated RML report for all packages, and removed some unnecessary files.
</commit_message>
<xml_diff>
--- a/mappings/package_F13/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F13/transformation/conceptual_mappings.xlsx
@@ -54,7 +54,7 @@
     <t>Mapping Version</t>
   </si>
   <si>
-    <t>6.5.0</t>
+    <t>6.6.0</t>
   </si>
   <si>
     <r>
@@ -133,7 +133,7 @@
     <t>Start Date</t>
   </si>
   <si>
-    <t>2020-10-08</t>
+    <t>2014-01-01</t>
   </si>
   <si>
     <t>one value, or empty cell</t>
@@ -145,7 +145,7 @@
     <t>Min XSD Version</t>
   </si>
   <si>
-    <t>R2.0.9.S03.E01</t>
+    <t>R2.0.9.S01.E01</t>
   </si>
   <si>
     <t>This fiels to be checked and updated if necessary</t>
@@ -5890,7 +5890,7 @@
       <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="20" t="s">

</xml_diff>